<commit_message>
Ready file is tested by run python scripts
</commit_message>
<xml_diff>
--- a/Python/Get_Iranian_Bank_Data/Iranian_Banks.xlsx
+++ b/Python/Get_Iranian_Bank_Data/Iranian_Banks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasma\Desktop\Kasma_Programming_Practice\Python\Get_Iranian_Bank_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FBE840-12AE-4F54-8D71-E9A4B9762B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B666A9-8881-437E-9558-97498E96C0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +383,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,13 +426,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,7 +746,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,7 +776,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -775,7 +790,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -792,7 +807,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
@@ -815,7 +830,7 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E5" t="s">
@@ -823,7 +838,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
@@ -840,7 +855,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
@@ -873,19 +888,19 @@
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
+      <c r="C9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
@@ -908,7 +923,7 @@
       <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E11" t="s">
@@ -916,7 +931,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B12" t="s">
@@ -930,7 +945,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
@@ -960,7 +975,7 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
@@ -977,7 +992,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B16" t="s">
@@ -994,7 +1009,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B17" t="s">
@@ -1011,7 +1026,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B18" t="s">
@@ -1028,7 +1043,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B19" t="s">
@@ -1045,7 +1060,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B20" t="s">
@@ -1062,7 +1077,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B21" t="s">
@@ -1079,7 +1094,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B22" t="s">
@@ -1096,7 +1111,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B23" t="s">
@@ -1113,7 +1128,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B24" t="s">
@@ -1130,7 +1145,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B25" t="s">
@@ -1147,7 +1162,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B26" t="s">
@@ -1164,7 +1179,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B27" t="s">
@@ -1181,7 +1196,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B28" t="s">

</xml_diff>